<commit_message>
Exercício desafio de portas lógicas
</commit_message>
<xml_diff>
--- a/Portas Lógicas Exercício 02 - Natália.xlsx
+++ b/Portas Lógicas Exercício 02 - Natália.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ADS\ADS_Automacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natália Nogueira\Desktop\ADS\ADS_Automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3762BB-B122-4ECA-97E4-D69919E979C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED797D13-75AC-480F-AB6C-AEA156630EF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="5" xr2:uid="{63589DE7-919D-4536-9115-0D92C656695E}"/>
   </bookViews>
@@ -342,66 +342,6 @@
         <a:xfrm>
           <a:off x="4330700" y="374650"/>
           <a:ext cx="4356100" cy="844550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E55C57-9794-4D69-B2BB-B0518B0CB86E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="21464"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3765550" y="374650"/>
-          <a:ext cx="4743450" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,66 +583,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06987C06-F3AA-4458-BF7C-C756EC8F878F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="23818"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4241800" y="368300"/>
-          <a:ext cx="4559300" cy="952500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -759,7 +639,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -819,7 +699,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -860,6 +740,66 @@
         <a:xfrm>
           <a:off x="4940300" y="355600"/>
           <a:ext cx="4540250" cy="920115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E55C57-9794-4D69-B2BB-B0518B0CB86E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="21464"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3765550" y="374650"/>
+          <a:ext cx="4743450" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1733,7 +1673,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1899,7 +1839,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1991,7 +1931,6 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>